<commit_message>
Adicionei a NN com uma saída (nn_dup)
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Assignment1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71F1CF99-9BE3-4EDA-AA1B-916BFF385794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F34406-03AA-4DCE-8B1C-E0423B5A1256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>Features</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>NN</t>
+  </si>
+  <si>
+    <t>SVM</t>
   </si>
 </sst>
 </file>
@@ -67,15 +70,33 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -83,13 +104,118 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -370,59 +496,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.21875" customWidth="1"/>
     <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="9">
         <v>0.94599999999999995</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="6">
         <v>0.95</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="8">
         <v>0.89700000000000002</v>
       </c>
-      <c r="D3">
-        <v>0.89700000000000002</v>
-      </c>
+      <c r="D3" s="7">
+        <v>0.89912499999999995</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I9" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Criei o arquivo 'dts.rar' com os datasets que vamos utilizar
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Assignment1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD0E3D1-5D36-4A20-BC65-547DB8E1B34A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3182AC3E-BB13-435E-9826-3FE887C9EF4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3396" yWindow="2016" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
-  <si>
-    <t>Features</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>Plain</t>
   </si>
@@ -76,6 +73,12 @@
   </si>
   <si>
     <t>Linear SVM</t>
+  </si>
+  <si>
+    <t>Obs</t>
+  </si>
+  <si>
+    <t>Select from model (logistic regression)</t>
   </si>
 </sst>
 </file>
@@ -666,10 +669,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -683,36 +686,36 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="E1" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>14</v>
-      </c>
       <c r="G1" s="2" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="35" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="16"/>
       <c r="C2" s="28"/>
@@ -720,7 +723,7 @@
       <c r="E2" s="28"/>
       <c r="F2" s="29"/>
       <c r="G2" s="7" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2" s="9">
         <v>0.94599999999999995</v>
@@ -737,7 +740,7 @@
       <c r="E3" s="25"/>
       <c r="F3" s="25"/>
       <c r="G3" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H3" s="4">
         <v>0.94699999999999995</v>
@@ -754,7 +757,7 @@
       <c r="E4" s="33"/>
       <c r="F4" s="28"/>
       <c r="G4" s="12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H4" s="4">
         <v>0.94499999999999995</v>
@@ -771,7 +774,7 @@
       <c r="E5" s="33"/>
       <c r="F5" s="34"/>
       <c r="G5" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H5" s="4">
         <v>0.97599999999999998</v>
@@ -802,82 +805,84 @@
       <c r="D7" s="24"/>
       <c r="E7" s="26"/>
       <c r="F7" s="27"/>
-      <c r="G7" s="12"/>
+      <c r="G7" s="12" t="s">
+        <v>17</v>
+      </c>
       <c r="H7" s="4">
-        <v>0.97799999999999998</v>
+        <v>0.99</v>
       </c>
       <c r="I7" s="12">
-        <v>0.98</v>
+        <v>0.98199999999999998</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="37"/>
+      <c r="A8" s="36"/>
       <c r="B8" s="16"/>
       <c r="C8" s="23"/>
       <c r="D8" s="24"/>
       <c r="E8" s="26"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="12" t="s">
-        <v>8</v>
-      </c>
+      <c r="F8" s="27"/>
+      <c r="G8" s="12"/>
       <c r="H8" s="4">
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="I8" s="12">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" s="37"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" s="4">
         <v>0.94299999999999995</v>
       </c>
-      <c r="I8" s="12">
+      <c r="I9" s="12">
         <v>0.95599999999999996</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="16"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H10" s="8">
+        <v>0.89700000000000002</v>
+      </c>
+      <c r="I10" s="7">
+        <v>0.89912499999999995</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H9" s="8">
-        <v>0.89700000000000002</v>
-      </c>
-      <c r="I9" s="7">
-        <v>0.89912499999999995</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="35" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="H10" s="4">
+      <c r="B11" s="16"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="H11" s="4">
         <v>0.97799999999999998</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I11" s="4">
         <v>0.97</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="36"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="4">
-        <v>0.73599999999999999</v>
-      </c>
-      <c r="I11" s="13">
-        <v>0.751</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
@@ -885,46 +890,78 @@
       <c r="B12" s="16"/>
       <c r="C12" s="23"/>
       <c r="D12" s="24"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="27"/>
       <c r="G12" s="12" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="H12" s="4">
-        <v>0.97299999999999998</v>
+        <v>0.99</v>
       </c>
       <c r="I12" s="13">
-        <v>0.96899999999999997</v>
+        <v>0.98199999999999998</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="21" t="s">
-        <v>16</v>
-      </c>
+      <c r="A13" s="36"/>
       <c r="B13" s="16"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="20"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="27"/>
       <c r="G13" s="12"/>
       <c r="H13" s="4">
+        <v>0.73599999999999999</v>
+      </c>
+      <c r="I13" s="13">
+        <v>0.751</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="36"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H14" s="4">
+        <v>0.97299999999999998</v>
+      </c>
+      <c r="I14" s="13">
+        <v>0.96899999999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="16"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="4">
         <v>0.95099999999999996</v>
       </c>
-      <c r="I13" s="13">
+      <c r="I15" s="13">
         <v>0.95</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="22"/>
-      <c r="N14" s="11"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" s="22"/>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="22"/>
+      <c r="N16" s="11"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="A11:A14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>